<commit_message>
Progress on integrating pLCI + maps of Canada CMs
</commit_message>
<xml_diff>
--- a/data/LCI/lci_LIB_raw_materials.xlsx
+++ b/data/LCI/lci_LIB_raw_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Data/Scientific_articles/decarbonization_LIB_raw_materials-v1.0/robyistrate-decarbonization_LIB_raw_materials-451e7ca/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/regional_minerals_sustainability/data/LCI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3005" documentId="13_ncr:1_{0CD9267C-230F-4C32-BDB0-E201BD3784C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85D9A1FB-F11C-43AC-9DEA-EF1CE753542A}"/>
+  <xr:revisionPtr revIDLastSave="3009" documentId="13_ncr:1_{0CD9267C-230F-4C32-BDB0-E201BD3784C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2F371B1-D19C-4C02-B1E4-E6989B65B22E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
@@ -2928,13 +2928,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2942,6 +2939,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2952,14 +2955,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3296,8 +3296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83C59EE-1777-41E4-AD79-BDA4CD03F3B5}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4944,7 +4944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6633,7 +6633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6877D36A-0BAC-4924-91DD-945153EBE883}">
   <dimension ref="A1:P173"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I55" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6793,7 +6795,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I10" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>716</v>
@@ -6824,7 +6826,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I11" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>716</v>
@@ -6855,7 +6857,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I12" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>716</v>
@@ -6888,7 +6890,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I13" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" t="s">
         <v>716</v>
@@ -6918,7 +6920,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I14" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="s">
         <v>716</v>
@@ -6948,7 +6950,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I15" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" t="s">
         <v>716</v>
@@ -6978,7 +6980,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I16" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>716</v>
@@ -7009,7 +7011,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I17" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>716</v>
@@ -7039,7 +7041,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I18" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" t="s">
         <v>716</v>
@@ -7072,7 +7074,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I19" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>716</v>
@@ -7106,7 +7108,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I20" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>716</v>
@@ -7137,7 +7139,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I21" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>716</v>
@@ -7168,7 +7170,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I22" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>716</v>
@@ -7345,7 +7347,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I33" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33" t="s">
         <v>716</v>
@@ -7376,7 +7378,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I34" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J34" t="s">
         <v>716</v>
@@ -7407,7 +7409,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I35" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35" t="s">
         <v>716</v>
@@ -7440,7 +7442,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I36" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
         <v>716</v>
@@ -7470,7 +7472,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I37" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" t="s">
         <v>716</v>
@@ -7500,7 +7502,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I38" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="s">
         <v>716</v>
@@ -7530,7 +7532,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I39" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39" t="s">
         <v>716</v>
@@ -7561,7 +7563,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I40" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J40" t="s">
         <v>716</v>
@@ -7591,7 +7593,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I41" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" t="s">
         <v>716</v>
@@ -7625,7 +7627,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I42" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
         <v>716</v>
@@ -7659,7 +7661,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I43" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
         <v>716</v>
@@ -7690,7 +7692,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I44" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
         <v>716</v>
@@ -7721,7 +7723,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I45" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
         <v>716</v>
@@ -7888,7 +7890,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I56" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J56" t="s">
         <v>714</v>
@@ -7921,7 +7923,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I57" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>714</v>
@@ -7951,7 +7953,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I58" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J58" t="s">
         <v>714</v>
@@ -7984,7 +7986,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I59" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J59" t="s">
         <v>714</v>
@@ -8017,7 +8019,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I60" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J60" t="s">
         <v>714</v>
@@ -8051,7 +8053,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I61" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J61" t="s">
         <v>714</v>
@@ -8081,7 +8083,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I62" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J62" t="s">
         <v>714</v>
@@ -8111,7 +8113,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I63" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J63" t="s">
         <v>714</v>
@@ -8142,7 +8144,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I64" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J64" t="s">
         <v>714</v>
@@ -8172,7 +8174,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I65" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J65" t="s">
         <v>714</v>
@@ -8203,7 +8205,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I66" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J66" t="s">
         <v>714</v>
@@ -8236,7 +8238,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I67" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J67" t="s">
         <v>714</v>
@@ -8269,7 +8271,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I68" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
         <v>714</v>
@@ -8299,7 +8301,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I69" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" t="s">
         <v>714</v>
@@ -8329,7 +8331,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I70" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J70" t="s">
         <v>714</v>
@@ -8359,7 +8361,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I71" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J71" t="s">
         <v>714</v>
@@ -8389,7 +8391,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I72" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J72" t="s">
         <v>714</v>
@@ -8421,7 +8423,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I73" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J73" t="s">
         <v>714</v>
@@ -8453,7 +8455,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I74" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J74" t="s">
         <v>714</v>
@@ -8485,7 +8487,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I75" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J75" t="s">
         <v>714</v>
@@ -8517,7 +8519,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I76" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J76" t="s">
         <v>714</v>
@@ -8550,7 +8552,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I77" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J77" t="s">
         <v>714</v>
@@ -8582,7 +8584,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I78" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J78" t="s">
         <v>714</v>
@@ -8614,7 +8616,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I79" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J79" t="s">
         <v>714</v>
@@ -8644,7 +8646,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I80" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J80" t="s">
         <v>714</v>
@@ -8676,7 +8678,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I81" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J81" t="s">
         <v>714</v>
@@ -8708,7 +8710,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I82" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J82" t="s">
         <v>714</v>
@@ -8740,7 +8742,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I83" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J83" t="s">
         <v>714</v>
@@ -8999,8 +9001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7526F10-A44B-4159-997F-0A6BAB3CF087}">
   <dimension ref="A1:XFA86"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I43" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15302,7 +15304,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I10" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="77" t="s">
         <v>770</v>
@@ -15332,7 +15334,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I11" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11" s="77" t="s">
         <v>770</v>
@@ -15363,7 +15365,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I12" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" s="77" t="s">
         <v>770</v>
@@ -15396,7 +15398,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I13" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" s="77" t="s">
         <v>770</v>
@@ -15426,7 +15428,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I14" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" s="77" t="s">
         <v>770</v>
@@ -15456,7 +15458,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I15" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" s="77" t="s">
         <v>770</v>
@@ -15486,7 +15488,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I16" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" s="77" t="s">
         <v>770</v>
@@ -15516,7 +15518,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I17" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" s="77" t="s">
         <v>770</v>
@@ -15546,7 +15548,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I18" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" s="77" t="s">
         <v>770</v>
@@ -15576,7 +15578,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I19" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19" s="77" t="s">
         <v>770</v>
@@ -15606,7 +15608,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I20" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" s="77" t="s">
         <v>770</v>
@@ -15636,7 +15638,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I21" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" s="77" t="s">
         <v>770</v>
@@ -15666,7 +15668,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I22" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" s="77" t="s">
         <v>770</v>
@@ -15696,7 +15698,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I23" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23" s="77" t="s">
         <v>770</v>
@@ -15726,7 +15728,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I24" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" s="77" t="s">
         <v>770</v>
@@ -15756,7 +15758,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I25" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25" s="77" t="s">
         <v>770</v>
@@ -15786,7 +15788,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I26" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26" s="77" t="s">
         <v>770</v>
@@ -15816,7 +15818,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I27" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" s="77" t="s">
         <v>770</v>
@@ -15846,7 +15848,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I28" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28" s="77" t="s">
         <v>770</v>
@@ -15873,7 +15875,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I29" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" s="77" t="s">
         <v>770</v>
@@ -15900,7 +15902,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I30" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J30" s="77" t="s">
         <v>770</v>
@@ -22269,7 +22271,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I41" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" s="75" t="s">
         <v>760</v>
@@ -22299,7 +22301,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I42" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42" s="75" t="s">
         <v>760</v>
@@ -22329,7 +22331,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I43" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
         <v>754</v>
@@ -22359,7 +22361,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I44" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
         <v>754</v>
@@ -22389,7 +22391,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I45" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
         <v>754</v>
@@ -22419,7 +22421,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I46" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J46" t="s">
         <v>754</v>
@@ -22449,7 +22451,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I47" s="75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47" s="75" t="s">
         <v>760</v>
@@ -22579,7 +22581,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I52" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J52" t="s">
         <v>754</v>
@@ -22606,7 +22608,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I53" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J53" t="s">
         <v>754</v>
@@ -28984,7 +28986,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I64" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>755</v>
@@ -29016,7 +29018,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I65" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J65" s="6" t="s">
         <v>755</v>
@@ -29047,7 +29049,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I66" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>755</v>
@@ -29074,7 +29076,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I67" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J67" s="6" t="s">
         <v>754</v>
@@ -29101,7 +29103,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I68" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>754</v>
@@ -29128,7 +29130,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I69" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" s="6" t="s">
         <v>754</v>
@@ -29168,8 +29170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A386841A-7D2F-44FE-BC7D-453E0B437B7D}">
   <dimension ref="A1:AS303"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView topLeftCell="A293" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I3" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29335,7 +29337,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I10" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>776</v>
@@ -29366,7 +29368,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I11" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>776</v>
@@ -29396,7 +29398,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I12" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>776</v>
@@ -29429,7 +29431,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I13" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" t="s">
         <v>776</v>
@@ -29462,7 +29464,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I14" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="s">
         <v>776</v>
@@ -29495,7 +29497,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I15" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" t="s">
         <v>776</v>
@@ -29528,7 +29530,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I16" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>776</v>
@@ -29561,7 +29563,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I17" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>776</v>
@@ -29591,7 +29593,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I18" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" t="s">
         <v>776</v>
@@ -29625,7 +29627,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I19" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>776</v>
@@ -29659,7 +29661,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I20" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>776</v>
@@ -29705,7 +29707,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I21" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>776</v>
@@ -29736,7 +29738,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I22" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>776</v>
@@ -29766,7 +29768,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I23" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>776</v>
@@ -29799,7 +29801,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I24" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
         <v>776</v>
@@ -29832,7 +29834,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I25" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25" t="s">
         <v>776</v>
@@ -29862,7 +29864,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I26" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26" t="s">
         <v>776</v>
@@ -29892,7 +29894,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I27" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" t="s">
         <v>776</v>
@@ -29922,7 +29924,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I28" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
         <v>776</v>
@@ -29952,7 +29954,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I29" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" t="s">
         <v>776</v>
@@ -29982,7 +29984,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I30" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J30" t="s">
         <v>776</v>
@@ -30012,7 +30014,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I31" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J31" t="s">
         <v>776</v>
@@ -30043,7 +30045,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I32" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J32" t="s">
         <v>776</v>
@@ -30076,7 +30078,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I33" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33" t="s">
         <v>776</v>
@@ -30106,7 +30108,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I34" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J34" t="s">
         <v>776</v>
@@ -30139,7 +30141,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I35" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35" t="s">
         <v>776</v>
@@ -30169,7 +30171,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I36" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
         <v>776</v>
@@ -30199,7 +30201,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I37" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" t="s">
         <v>776</v>
@@ -30229,7 +30231,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I38" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="s">
         <v>776</v>
@@ -30262,7 +30264,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I39" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39" t="s">
         <v>776</v>
@@ -30292,7 +30294,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I40" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J40" t="s">
         <v>776</v>
@@ -30325,7 +30327,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I41" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" t="s">
         <v>776</v>
@@ -30355,7 +30357,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I42" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
         <v>776</v>
@@ -30385,7 +30387,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I43" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
         <v>776</v>
@@ -30415,7 +30417,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I44" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
         <v>776</v>
@@ -30449,7 +30451,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I45" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
         <v>776</v>
@@ -30495,7 +30497,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I46" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J46" t="s">
         <v>776</v>
@@ -30528,7 +30530,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I47" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47" t="s">
         <v>776</v>
@@ -30561,7 +30563,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I48" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J48" t="s">
         <v>776</v>
@@ -30591,7 +30593,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I49" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J49" t="s">
         <v>776</v>
@@ -30618,7 +30620,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I50" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J50" t="s">
         <v>776</v>
@@ -30645,7 +30647,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I51" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J51" t="s">
         <v>776</v>
@@ -30672,7 +30674,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I52" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J52" t="s">
         <v>776</v>
@@ -30699,7 +30701,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I53" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J53" t="s">
         <v>776</v>
@@ -30726,7 +30728,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I54" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J54" t="s">
         <v>776</v>
@@ -30753,7 +30755,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I55" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J55" t="s">
         <v>776</v>
@@ -30780,7 +30782,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I56" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J56" t="s">
         <v>776</v>
@@ -30807,7 +30809,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I57" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>776</v>
@@ -30834,7 +30836,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I58" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J58" t="s">
         <v>776</v>
@@ -30861,7 +30863,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I59" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J59" t="s">
         <v>776</v>
@@ -30888,7 +30890,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I60" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J60" t="s">
         <v>776</v>
@@ -30915,7 +30917,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I61" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J61" t="s">
         <v>776</v>
@@ -30942,7 +30944,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I62" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J62" t="s">
         <v>776</v>
@@ -30969,7 +30971,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I63" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J63" t="s">
         <v>776</v>
@@ -30996,7 +30998,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I64" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J64" t="s">
         <v>776</v>
@@ -31023,7 +31025,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I65" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J65" t="s">
         <v>776</v>
@@ -31050,7 +31052,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I66" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J66" t="s">
         <v>776</v>
@@ -31077,7 +31079,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I67" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J67" t="s">
         <v>776</v>
@@ -31104,7 +31106,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I68" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
         <v>776</v>
@@ -31131,7 +31133,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I69" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" t="s">
         <v>776</v>
@@ -31158,7 +31160,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I70" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J70" t="s">
         <v>776</v>
@@ -31185,7 +31187,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I71" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J71" t="s">
         <v>776</v>
@@ -31212,7 +31214,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I72" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J72" t="s">
         <v>776</v>
@@ -31239,7 +31241,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I73" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J73" t="s">
         <v>776</v>
@@ -31266,7 +31268,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I74" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J74" t="s">
         <v>776</v>
@@ -31293,7 +31295,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I75" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J75" t="s">
         <v>776</v>
@@ -31320,7 +31322,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I76" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J76" t="s">
         <v>776</v>
@@ -31347,7 +31349,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I77" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J77" t="s">
         <v>776</v>
@@ -31374,7 +31376,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I78" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J78" t="s">
         <v>776</v>
@@ -31543,7 +31545,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I89" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J89" t="s">
         <v>776</v>
@@ -31573,7 +31575,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I90" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J90" t="s">
         <v>776</v>
@@ -31604,7 +31606,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I91" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J91" t="s">
         <v>776</v>
@@ -31638,7 +31640,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I92" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J92" t="s">
         <v>776</v>
@@ -31674,7 +31676,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I93" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J93" t="s">
         <v>776</v>
@@ -31710,7 +31712,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I94" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J94" t="s">
         <v>776</v>
@@ -31745,7 +31747,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I95" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J95" t="s">
         <v>776</v>
@@ -31776,7 +31778,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I96" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J96" t="s">
         <v>776</v>
@@ -31807,7 +31809,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I97" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J97" t="s">
         <v>776</v>
@@ -31838,7 +31840,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I98" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J98" t="s">
         <v>776</v>
@@ -31869,7 +31871,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I99" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J99" t="s">
         <v>776</v>
@@ -31903,7 +31905,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I100" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J100" t="s">
         <v>776</v>
@@ -31936,7 +31938,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I101" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J101" t="s">
         <v>776</v>
@@ -31969,7 +31971,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I102" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J102" t="s">
         <v>776</v>
@@ -32002,7 +32004,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I103" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J103" t="s">
         <v>776</v>
@@ -32032,7 +32034,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I104" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
         <v>776</v>
@@ -32062,7 +32064,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I105" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
         <v>776</v>
@@ -32095,7 +32097,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I106" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J106" t="s">
         <v>776</v>
@@ -32128,7 +32130,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I107" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J107" t="s">
         <v>776</v>
@@ -32158,7 +32160,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I108" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J108" t="s">
         <v>776</v>
@@ -32191,7 +32193,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I109" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J109" t="s">
         <v>776</v>
@@ -32221,7 +32223,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I110" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J110" t="s">
         <v>776</v>
@@ -32251,7 +32253,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I111" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J111" t="s">
         <v>776</v>
@@ -32281,7 +32283,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I112" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J112" t="s">
         <v>776</v>
@@ -32314,7 +32316,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I113" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J113" t="s">
         <v>776</v>
@@ -32347,7 +32349,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I114" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J114" t="s">
         <v>776</v>
@@ -32377,7 +32379,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I115" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J115" t="s">
         <v>776</v>
@@ -32410,7 +32412,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I116" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J116" t="s">
         <v>776</v>
@@ -32440,7 +32442,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I117" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J117" t="s">
         <v>776</v>
@@ -32473,7 +32475,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I118" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J118" t="s">
         <v>776</v>
@@ -32503,7 +32505,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I119" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J119" t="s">
         <v>776</v>
@@ -32533,7 +32535,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I120" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J120" t="s">
         <v>776</v>
@@ -32563,7 +32565,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I121" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J121" t="s">
         <v>776</v>
@@ -32596,7 +32598,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I122" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J122" t="s">
         <v>776</v>
@@ -32626,7 +32628,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I123" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J123" t="s">
         <v>776</v>
@@ -32656,7 +32658,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I124" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J124" t="s">
         <v>776</v>
@@ -32689,7 +32691,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I125" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J125" t="s">
         <v>776</v>
@@ -32722,7 +32724,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I126" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J126" t="s">
         <v>776</v>
@@ -32755,7 +32757,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I127" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J127" t="s">
         <v>776</v>
@@ -32788,7 +32790,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I128" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J128" t="s">
         <v>776</v>
@@ -32818,7 +32820,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I129" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J129" t="s">
         <v>776</v>
@@ -32848,7 +32850,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I130" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J130" t="s">
         <v>776</v>
@@ -32879,7 +32881,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I131" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J131" t="s">
         <v>776</v>
@@ -32906,7 +32908,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I132" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J132" t="s">
         <v>776</v>
@@ -32933,7 +32935,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I133" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J133" t="s">
         <v>776</v>
@@ -32960,7 +32962,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I134" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J134" t="s">
         <v>776</v>
@@ -32987,7 +32989,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I135" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J135" t="s">
         <v>776</v>
@@ -33017,7 +33019,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I136" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J136" t="s">
         <v>776</v>
@@ -33044,7 +33046,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I137" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J137" t="s">
         <v>776</v>
@@ -33071,7 +33073,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I138" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J138" t="s">
         <v>776</v>
@@ -33101,7 +33103,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I139" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J139" t="s">
         <v>776</v>
@@ -33128,7 +33130,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I140" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J140" t="s">
         <v>776</v>
@@ -33155,7 +33157,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I141" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J141" t="s">
         <v>776</v>
@@ -33182,7 +33184,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I142" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J142" t="s">
         <v>776</v>
@@ -33210,7 +33212,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I143" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J143" t="s">
         <v>776</v>
@@ -33238,7 +33240,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I144" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J144" t="s">
         <v>776</v>
@@ -33266,7 +33268,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I145" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J145" t="s">
         <v>776</v>
@@ -33294,7 +33296,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I146" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J146" t="s">
         <v>776</v>
@@ -33322,7 +33324,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I147" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J147" t="s">
         <v>776</v>
@@ -33350,7 +33352,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I148" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J148" t="s">
         <v>776</v>
@@ -33377,7 +33379,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I149" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J149" t="s">
         <v>776</v>
@@ -33405,7 +33407,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I150" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J150" t="s">
         <v>776</v>
@@ -33433,7 +33435,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I151" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J151" t="s">
         <v>776</v>
@@ -33461,7 +33463,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I152" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J152" t="s">
         <v>776</v>
@@ -33488,7 +33490,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I153" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J153" t="s">
         <v>776</v>
@@ -33515,7 +33517,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I154" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J154" t="s">
         <v>776</v>
@@ -33542,7 +33544,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I155" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J155" t="s">
         <v>776</v>
@@ -33569,7 +33571,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I156" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J156" t="s">
         <v>776</v>
@@ -33596,7 +33598,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I157" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J157" t="s">
         <v>776</v>
@@ -33623,7 +33625,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I158" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J158" t="s">
         <v>776</v>
@@ -33650,7 +33652,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I159" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J159" t="s">
         <v>776</v>
@@ -33839,7 +33841,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I170" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J170" t="s">
         <v>776</v>
@@ -33869,7 +33871,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I171" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J171" t="s">
         <v>776</v>
@@ -33900,7 +33902,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I172" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J172" t="s">
         <v>776</v>
@@ -33933,7 +33935,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I173" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J173" t="s">
         <v>776</v>
@@ -33966,7 +33968,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I174" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J174" t="s">
         <v>776</v>
@@ -33999,7 +34001,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I175" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J175" t="s">
         <v>776</v>
@@ -34032,7 +34034,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I176" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J176" t="s">
         <v>776</v>
@@ -34066,7 +34068,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I177" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J177" t="s">
         <v>776</v>
@@ -34099,7 +34101,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I178" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J178" t="s">
         <v>776</v>
@@ -34132,7 +34134,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I179" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J179" t="s">
         <v>776</v>
@@ -34165,7 +34167,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I180" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J180" t="s">
         <v>776</v>
@@ -34198,7 +34200,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I181" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J181" t="s">
         <v>776</v>
@@ -34228,7 +34230,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I182" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J182" t="s">
         <v>776</v>
@@ -34261,7 +34263,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I183" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J183" t="s">
         <v>776</v>
@@ -34294,7 +34296,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I184" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J184" t="s">
         <v>776</v>
@@ -34327,7 +34329,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I185" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J185" t="s">
         <v>776</v>
@@ -34357,7 +34359,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I186" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J186" t="s">
         <v>776</v>
@@ -34390,7 +34392,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I187" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J187" t="s">
         <v>776</v>
@@ -34423,7 +34425,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I188" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J188" t="s">
         <v>776</v>
@@ -34456,7 +34458,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I189" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J189" t="s">
         <v>776</v>
@@ -34489,7 +34491,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I190" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J190" t="s">
         <v>776</v>
@@ -34522,7 +34524,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I191" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J191" t="s">
         <v>776</v>
@@ -34552,7 +34554,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I192" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J192" t="s">
         <v>776</v>
@@ -34582,7 +34584,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I193" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J193" t="s">
         <v>776</v>
@@ -34612,7 +34614,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I194" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J194" t="s">
         <v>776</v>
@@ -34642,7 +34644,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I195" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J195" t="s">
         <v>776</v>
@@ -34669,7 +34671,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I196" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J196" t="s">
         <v>776</v>
@@ -34696,7 +34698,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I197" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J197" t="s">
         <v>776</v>
@@ -34726,7 +34728,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I198" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J198" t="s">
         <v>776</v>
@@ -34753,7 +34755,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I199" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J199" t="s">
         <v>776</v>
@@ -34780,7 +34782,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I200" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J200" t="s">
         <v>776</v>
@@ -34807,7 +34809,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I201" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J201" t="s">
         <v>776</v>
@@ -34989,7 +34991,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I212" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J212" t="s">
         <v>776</v>
@@ -35023,7 +35025,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I213" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J213" t="s">
         <v>776</v>
@@ -35056,7 +35058,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I214" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J214" t="s">
         <v>776</v>
@@ -35089,7 +35091,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I215" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J215" t="s">
         <v>776</v>
@@ -35123,7 +35125,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I216" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J216" t="s">
         <v>776</v>
@@ -35156,7 +35158,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I217" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J217" t="s">
         <v>776</v>
@@ -35189,7 +35191,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I218" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J218" t="s">
         <v>776</v>
@@ -35222,7 +35224,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I219" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J219" t="s">
         <v>776</v>
@@ -35255,7 +35257,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I220" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J220" t="s">
         <v>776</v>
@@ -35288,7 +35290,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I221" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J221" t="s">
         <v>776</v>
@@ -35321,7 +35323,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I222" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J222" t="s">
         <v>776</v>
@@ -35351,7 +35353,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I223" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J223" t="s">
         <v>776</v>
@@ -35381,7 +35383,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I224" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J224" t="s">
         <v>776</v>
@@ -35411,7 +35413,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I225" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J225" t="s">
         <v>776</v>
@@ -35441,7 +35443,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I226" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J226" t="s">
         <v>776</v>
@@ -35471,7 +35473,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I227" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J227" t="s">
         <v>776</v>
@@ -35501,7 +35503,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I228" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J228" t="s">
         <v>776</v>
@@ -35531,7 +35533,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I229" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J229" t="s">
         <v>776</v>
@@ -35561,7 +35563,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I230" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J230" t="s">
         <v>776</v>
@@ -35591,7 +35593,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I231" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J231" t="s">
         <v>776</v>
@@ -35621,7 +35623,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I232" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J232" t="s">
         <v>776</v>
@@ -35648,7 +35650,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I233" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J233" t="s">
         <v>776</v>
@@ -35675,7 +35677,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I234" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J234" t="s">
         <v>776</v>
@@ -35702,7 +35704,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I235" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J235" t="s">
         <v>776</v>
@@ -35729,7 +35731,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I236" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J236" t="s">
         <v>776</v>
@@ -35759,7 +35761,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I237" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J237" t="s">
         <v>776</v>
@@ -35786,7 +35788,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I238" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J238" t="s">
         <v>776</v>
@@ -35813,7 +35815,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I239" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J239" t="s">
         <v>776</v>
@@ -35840,7 +35842,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I240" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J240" t="s">
         <v>776</v>
@@ -35867,7 +35869,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I241" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J241" t="s">
         <v>776</v>
@@ -35894,7 +35896,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I242" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J242" t="s">
         <v>776</v>
@@ -37175,8 +37177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3D24D4-2E6F-41D5-89DB-3F789653CF27}">
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39324,8 +39326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024CCAE1-AADE-4D85-A6C2-DF07BF45D505}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71:J74"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39537,7 +39539,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I10" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>732</v>
@@ -39572,7 +39574,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I11" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>733</v>
@@ -39607,7 +39609,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I12" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>732</v>
@@ -39644,7 +39646,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I13" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" t="s">
         <v>733</v>
@@ -39681,7 +39683,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I14" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="s">
         <v>733</v>
@@ -39719,7 +39721,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I15" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" t="s">
         <v>733</v>
@@ -39757,7 +39759,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I16" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>733</v>
@@ -39794,7 +39796,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I17" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>732</v>
@@ -40009,7 +40011,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I28" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
         <v>733</v>
@@ -40046,7 +40048,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I29" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" t="s">
         <v>732</v>
@@ -40083,7 +40085,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I30" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J30" t="s">
         <v>733</v>
@@ -40302,7 +40304,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I41" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" t="s">
         <v>732</v>
@@ -40338,7 +40340,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I42" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
         <v>732</v>
@@ -40373,7 +40375,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I43" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
         <v>732</v>
@@ -40407,7 +40409,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I44" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
         <v>733</v>
@@ -40444,7 +40446,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I45" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
         <v>732</v>
@@ -40477,7 +40479,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I46" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J46" t="s">
         <v>732</v>
@@ -40692,7 +40694,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I57" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>741</v>
@@ -40728,7 +40730,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I58" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J58" t="s">
         <v>741</v>
@@ -40762,7 +40764,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I59" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J59" t="s">
         <v>739</v>
@@ -40797,7 +40799,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I60" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J60" t="s">
         <v>743</v>
@@ -40830,7 +40832,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I61" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J61" t="s">
         <v>743</v>
@@ -40863,7 +40865,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I62" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J62" t="s">
         <v>743</v>
@@ -41078,7 +41080,7 @@
         <v>LIB raw materials</v>
       </c>
       <c r="I73" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J73" t="s">
         <v>732</v>
@@ -41115,7 +41117,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I74" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J74" t="s">
         <v>733</v>
@@ -41152,7 +41154,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I75" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J75" t="s">
         <v>733</v>
@@ -41371,7 +41373,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I86" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J86" t="s">
         <v>728</v>
@@ -41408,7 +41410,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I87" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J87" t="s">
         <v>728</v>
@@ -41445,7 +41447,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I88" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J88" t="s">
         <v>728</v>
@@ -41480,7 +41482,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I89" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J89" t="s">
         <v>728</v>
@@ -41515,7 +41517,7 @@
         <v>ecoinvent-3.10-cutoff</v>
       </c>
       <c r="I90" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J90" t="s">
         <v>728</v>
@@ -41548,7 +41550,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I91" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J91" t="s">
         <v>728</v>
@@ -41581,7 +41583,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I92" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J92" t="s">
         <v>728</v>
@@ -41612,7 +41614,7 @@
         <v>ecoinvent-3.10-biosphere</v>
       </c>
       <c r="I93" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J93" t="s">
         <v>728</v>
@@ -41634,7 +41636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B0F318-8C53-4B11-8704-083389C4343A}">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -42925,7 +42927,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
@@ -42983,10 +42985,10 @@
       <c r="K5" s="62"/>
     </row>
     <row r="6" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>695</v>
       </c>
       <c r="C6" s="70" t="s">
@@ -43012,8 +43014,8 @@
       <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" s="63" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="87"/>
-      <c r="B7" s="88"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="66" t="s">
         <v>701</v>
       </c>
@@ -43037,10 +43039,10 @@
       <c r="K7" s="62"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="92" t="s">
         <v>226</v>
       </c>
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="86" t="s">
         <v>695</v>
       </c>
       <c r="C8" s="70" t="s">
@@ -43063,8 +43065,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="66" t="s">
         <v>701</v>
       </c>
@@ -43085,8 +43087,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="92"/>
-      <c r="B10" s="88" t="s">
+      <c r="A10" s="93"/>
+      <c r="B10" s="86" t="s">
         <v>698</v>
       </c>
       <c r="C10" s="70" t="s">
@@ -43109,8 +43111,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="92"/>
-      <c r="B11" s="88"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="66" t="s">
         <v>701</v>
       </c>
@@ -43131,8 +43133,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="92"/>
-      <c r="B12" s="88" t="s">
+      <c r="A12" s="93"/>
+      <c r="B12" s="86" t="s">
         <v>191</v>
       </c>
       <c r="C12" s="70" t="s">
@@ -43155,8 +43157,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="93"/>
-      <c r="B13" s="88"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="66" t="s">
         <v>701</v>
       </c>
@@ -43177,10 +43179,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="88" t="s">
         <v>469</v>
       </c>
       <c r="C14" s="70" t="s">
@@ -43203,8 +43205,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="92"/>
-      <c r="B15" s="90"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="89"/>
       <c r="C15" s="66" t="s">
         <v>701</v>
       </c>
@@ -43225,8 +43227,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="92"/>
-      <c r="B16" s="95" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="90" t="s">
         <v>471</v>
       </c>
       <c r="C16" s="70" t="s">
@@ -43249,8 +43251,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="92"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="66" t="s">
         <v>701</v>
       </c>
@@ -43271,8 +43273,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="92"/>
-      <c r="B18" s="95" t="s">
+      <c r="A18" s="93"/>
+      <c r="B18" s="90" t="s">
         <v>472</v>
       </c>
       <c r="C18" s="70" t="s">
@@ -43295,8 +43297,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="93"/>
-      <c r="B19" s="96"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="91"/>
       <c r="C19" s="66" t="s">
         <v>701</v>
       </c>
@@ -43318,10 +43320,10 @@
       <c r="K19" s="77"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="90" t="s">
         <v>722</v>
       </c>
       <c r="C20" s="70" t="s">
@@ -43345,8 +43347,8 @@
       <c r="K20" s="77"/>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="93"/>
-      <c r="B21" s="96"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="66" t="s">
         <v>701</v>
       </c>
@@ -43368,10 +43370,10 @@
       <c r="K21" s="77"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="87" t="s">
         <v>721</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="88" t="s">
         <v>511</v>
       </c>
       <c r="C22" s="70" t="s">
@@ -43394,8 +43396,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="94"/>
-      <c r="B23" s="90"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="89"/>
       <c r="C23" s="66" t="s">
         <v>701</v>
       </c>
@@ -43417,8 +43419,8 @@
       <c r="K23" s="74"/>
     </row>
     <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="94"/>
-      <c r="B24" s="89" t="s">
+      <c r="A24" s="87"/>
+      <c r="B24" s="88" t="s">
         <v>483</v>
       </c>
       <c r="C24" s="70" t="s">
@@ -43441,8 +43443,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="94"/>
-      <c r="B25" s="90"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="89"/>
       <c r="C25" s="66" t="s">
         <v>701</v>
       </c>
@@ -43463,8 +43465,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="94"/>
-      <c r="B26" s="88" t="s">
+      <c r="A26" s="87"/>
+      <c r="B26" s="86" t="s">
         <v>520</v>
       </c>
       <c r="C26" s="70" t="s">
@@ -43487,8 +43489,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="94"/>
-      <c r="B27" s="88"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="66" t="s">
         <v>701</v>
       </c>
@@ -43509,8 +43511,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="94"/>
-      <c r="B28" s="88" t="s">
+      <c r="A28" s="87"/>
+      <c r="B28" s="86" t="s">
         <v>486</v>
       </c>
       <c r="C28" s="70" t="s">
@@ -43533,8 +43535,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="94"/>
-      <c r="B29" s="88"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="66" t="s">
         <v>701</v>
       </c>
@@ -43555,8 +43557,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="94"/>
-      <c r="B30" s="88" t="s">
+      <c r="A30" s="87"/>
+      <c r="B30" s="86" t="s">
         <v>487</v>
       </c>
       <c r="C30" s="70" t="s">
@@ -43579,8 +43581,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="94"/>
-      <c r="B31" s="88"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="66" t="s">
         <v>701</v>
       </c>
@@ -43601,8 +43603,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="94"/>
-      <c r="B32" s="88" t="s">
+      <c r="A32" s="87"/>
+      <c r="B32" s="86" t="s">
         <v>490</v>
       </c>
       <c r="C32" s="70" t="s">
@@ -43625,8 +43627,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="94"/>
-      <c r="B33" s="88"/>
+      <c r="A33" s="87"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="66" t="s">
         <v>701</v>
       </c>
@@ -43648,6 +43650,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A8:A13"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="A22:A33"/>
     <mergeCell ref="B14:B15"/>
@@ -43659,14 +43669,6 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A8:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>